<commit_message>
update the function insert product
</commit_message>
<xml_diff>
--- a/Document/ProductName-HoaCa.xlsx
+++ b/Document/ProductName-HoaCa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\iProjects\blogs\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F827D0-789A-4CB1-AD16-EFD4396C004E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBAE5A2-7055-4B5B-A648-E3BF17E8C2F6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210" tabRatio="804" activeTab="5" xr2:uid="{A9407308-5E89-47A8-B11F-33EC6B0F3C93}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="804" activeTab="5" xr2:uid="{A9407308-5E89-47A8-B11F-33EC6B0F3C93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -990,13 +990,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>85000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>38000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>166</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1211,7 +1211,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1225,12 +1225,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1577,12 +1577,12 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -1721,12 +1721,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -1849,13 +1849,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1918,13 +1918,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -2257,13 +2257,13 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -2432,12 +2432,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>94</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>103</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -2786,12 +2786,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3134,14 +3134,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>700-1tr000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E9" s="3" t="s">
         <v>171</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>165</v>
       </c>

</xml_diff>